<commit_message>
Testliste aktualisiert. Hibernate auf Update gesetzt.
</commit_message>
<xml_diff>
--- a/Stundenplan-DB/Dokumente/stundenplandb_testliste.xlsx
+++ b/Stundenplan-DB/Dokumente/stundenplandb_testliste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
   <si>
     <t>Lfd. Nr</t>
   </si>
@@ -199,12 +199,6 @@
   </si>
   <si>
     <t>Problem</t>
-  </si>
-  <si>
-    <t>Kollisionsmeldungen werden angezeigt, update funktioniert aber</t>
-  </si>
-  <si>
-    <t>Fehlermeldung Raum ist zu klein für Zenturie, stimmt aber nicht</t>
   </si>
   <si>
     <t>Es werden Kollisionsmeldungen für Dozent, Zenturie und Raum ausgegeben.</t>
@@ -298,7 +292,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,13 +308,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,7 +316,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,11 +326,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -365,24 +347,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -392,9 +370,8 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
-    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -697,8 +674,8 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,26 +840,26 @@
         <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f>A9+1</f>
         <v>9</v>
@@ -896,10 +873,8 @@
       <c r="D12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -915,10 +890,8 @@
       <c r="D13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -932,7 +905,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" s="4"/>
     </row>
@@ -941,14 +914,14 @@
         <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f>A14+1</f>
         <v>12</v>
@@ -962,23 +935,21 @@
       <c r="D16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1008,7 +979,7 @@
         <v>28</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" s="4"/>
     </row>
@@ -1017,10 +988,10 @@
         <v>30</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E20" s="4"/>
     </row>
@@ -1038,23 +1009,21 @@
       <c r="D21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -1065,7 +1034,7 @@
         <v>31</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -1081,10 +1050,10 @@
         <v>33</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" s="4"/>
     </row>
@@ -1093,14 +1062,14 @@
         <v>33</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f>A24+1</f>
         <v>18</v>
@@ -1114,23 +1083,21 @@
       <c r="D26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="6"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
@@ -1138,13 +1105,13 @@
         <v>19</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="E28" s="4"/>
     </row>
@@ -1154,13 +1121,13 @@
         <v>20</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="E29" s="4"/>
     </row>
@@ -1170,13 +1137,13 @@
         <v>21</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E30" s="4"/>
     </row>
@@ -1195,7 +1162,7 @@
         <v>38</v>
       </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="6"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -1212,7 +1179,7 @@
         <v>41</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="F32" s="7"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -1229,7 +1196,7 @@
         <v>49</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="6"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
@@ -1246,7 +1213,7 @@
         <v>52</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="6"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3">

</xml_diff>